<commit_message>
Week 3 Plan update
</commit_message>
<xml_diff>
--- a/Plan/Plan.xlsx
+++ b/Plan/Plan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Unity得分顯示</t>
   </si>
@@ -91,6 +91,36 @@
   </si>
   <si>
     <t>Y. 08 April 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">battlefield controller </t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>使用item需要的piece和現儲存的piece顯示</t>
+  </si>
+  <si>
+    <t>monster的技能設計</t>
+  </si>
+  <si>
+    <t>monster下回合行動提示</t>
+  </si>
+  <si>
+    <t>player的 green action改爲2piece攻擊1次，餘數再加一次流血debuff</t>
+  </si>
+  <si>
+    <t>player道具效果設計</t>
+  </si>
+  <si>
+    <t>設計</t>
+  </si>
+  <si>
+    <t>item效果實現</t>
+  </si>
+  <si>
+    <t>monster技能實現+隨機</t>
   </si>
 </sst>
 </file>
@@ -114,7 +144,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -223,11 +253,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -291,6 +332,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -586,24 +639,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="15" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="50.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.140625" style="5" customWidth="1"/>
     <col min="5" max="5" width="40.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="13.85546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="1"/>
       <c r="B1" s="7"/>
       <c r="C1" s="19" t="s">
@@ -614,8 +668,12 @@
         <v>3</v>
       </c>
       <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="19"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="20" t="s">
         <v>7</v>
       </c>
@@ -635,7 +693,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30">
+    <row r="3" spans="1:8" ht="30">
       <c r="A3" s="21"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12" t="s">
@@ -651,7 +709,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30">
+    <row r="4" spans="1:8" ht="30">
       <c r="A4" s="21"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12" t="s">
@@ -663,7 +721,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8">
       <c r="A5" s="21"/>
       <c r="B5" s="13">
         <v>43549</v>
@@ -677,7 +735,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6" s="21"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12" t="s">
@@ -687,7 +745,7 @@
       <c r="E6" s="12"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8">
       <c r="A7" s="21"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12" t="s">
@@ -697,7 +755,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8">
       <c r="A8" s="14"/>
       <c r="B8" s="14"/>
       <c r="C8" s="14" t="s">
@@ -706,8 +764,10 @@
       <c r="D8" s="15"/>
       <c r="E8" s="14"/>
       <c r="F8" s="15"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="25"/>
+      <c r="H8" s="14"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -723,9 +783,11 @@
       <c r="E9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="F9" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
@@ -735,18 +797,25 @@
       <c r="E10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="F10" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="E11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
@@ -755,7 +824,7 @@
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:8">
       <c r="B13" s="3">
         <v>43565</v>
       </c>
@@ -767,71 +836,108 @@
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:8">
       <c r="D14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:8">
       <c r="D15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6">
-      <c r="D16" s="4"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="4:6">
+    <row r="16" spans="1:8">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" ht="45">
+      <c r="B17" s="3">
+        <v>43576</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="D17" s="4"/>
+      <c r="E17" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="4:6">
+      <c r="G17" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45">
+      <c r="A18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>30</v>
+      </c>
       <c r="D18" s="4"/>
+      <c r="E18" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="4:6">
+      <c r="G18" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="48.75" customHeight="1">
+      <c r="C19" s="22" t="s">
+        <v>34</v>
+      </c>
       <c r="D19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="4:6">
+    <row r="20" spans="1:7">
       <c r="D20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="4:6">
+    <row r="21" spans="1:7">
+      <c r="B21" s="3">
+        <v>43584</v>
+      </c>
       <c r="D21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="4:6">
+    <row r="22" spans="1:7">
       <c r="D22" s="4"/>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="4:6">
+    <row r="23" spans="1:7">
       <c r="D23" s="4"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="4:6">
+    <row r="24" spans="1:7">
       <c r="D24" s="4"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="4:6">
+    <row r="25" spans="1:7">
       <c r="D25" s="4"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="4:6">
+    <row r="26" spans="1:7">
       <c r="D26" s="4"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="4:6">
+    <row r="27" spans="1:7">
       <c r="D27" s="4"/>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" spans="4:6">
+    <row r="28" spans="1:7">
       <c r="D28" s="4"/>
       <c r="F28" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A2:A7"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>